<commit_message>
thor-min_w and bias-indicator testing
</commit_message>
<xml_diff>
--- a/results_files/bnn_summary.xlsx
+++ b/results_files/bnn_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandonalston/Desktop/Code/BNN/results_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65633894-9FD3-4844-BCBD-D064B99A423B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A562EB4D-23E9-1F4C-9391-2BF900A1F98F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16320" xr2:uid="{E74465CE-9C89-6447-9368-51D7CC14DA8E}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -256,21 +256,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -19695,7 +19694,436 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A432F82B-CF35-A74B-AAA0-B4F9F7278C4A}" name="PivotTable7" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{26780794-9D53-6B4F-A2D3-003FF38CA31F}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="AW2:BG15" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
+      <items count="11">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="2"/>
+        <item x="9"/>
+        <item x="3"/>
+        <item x="10"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="5"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="6"/>
+    <field x="7"/>
+  </colFields>
+  <colItems count="10">
+    <i>
+      <x v="2"/>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Out-Acc" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B52A05F5-4A2D-2F47-BCE3-4E0F6ED46934}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="AG2:AQ15" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
+      <items count="11">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="2"/>
+        <item x="9"/>
+        <item x="3"/>
+        <item x="10"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="5"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="6"/>
+    <field x="7"/>
+  </colFields>
+  <colItems count="10">
+    <i>
+      <x v="2"/>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of In-Acc" fld="2" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{60EEC3AA-C79F-634E-A332-D68B06F3D76E}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="Q2:AA15" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
+      <items count="11">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="2"/>
+        <item x="9"/>
+        <item x="3"/>
+        <item x="10"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="5"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="6"/>
+    <field x="7"/>
+  </colFields>
+  <colItems count="10">
+    <i>
+      <x v="2"/>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Run_Time" fld="4" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A432F82B-CF35-A74B-AAA0-B4F9F7278C4A}" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="AW18:BG31" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -19837,8 +20265,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EF93F0E1-3217-AF4B-AC71-39BBDB260F95}" name="PivotTable6" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EF93F0E1-3217-AF4B-AC71-39BBDB260F95}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="AG18:AQ31" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -19980,8 +20408,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FBE3ADB6-1D72-F544-BCE7-349600E45F5D}" name="PivotTable5" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FBE3ADB6-1D72-F544-BCE7-349600E45F5D}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="Q18:AA31" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -20110,435 +20538,6 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Average of ObjVal" fld="11" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{26780794-9D53-6B4F-A2D3-003FF38CA31F}" name="PivotTable4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="AW2:BG15" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="13">
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
-      <items count="11">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="2"/>
-        <item x="9"/>
-        <item x="3"/>
-        <item x="10"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="6">
-        <item m="1" x="4"/>
-        <item m="1" x="5"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="6">
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="5"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="6"/>
-    <field x="7"/>
-  </colFields>
-  <colItems count="10">
-    <i>
-      <x v="2"/>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="4"/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="5"/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Out-Acc" fld="3" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B52A05F5-4A2D-2F47-BCE3-4E0F6ED46934}" name="PivotTable3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="AG2:AQ15" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="13">
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
-      <items count="11">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="2"/>
-        <item x="9"/>
-        <item x="3"/>
-        <item x="10"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="6">
-        <item m="1" x="4"/>
-        <item m="1" x="5"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="6">
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="5"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="6"/>
-    <field x="7"/>
-  </colFields>
-  <colItems count="10">
-    <i>
-      <x v="2"/>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="4"/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="5"/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of In-Acc" fld="2" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{60EEC3AA-C79F-634E-A332-D68B06F3D76E}" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="Q2:AA15" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="13">
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
-      <items count="11">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="2"/>
-        <item x="9"/>
-        <item x="3"/>
-        <item x="10"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="6">
-        <item m="1" x="4"/>
-        <item m="1" x="5"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="6">
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="5"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="6"/>
-    <field x="7"/>
-  </colFields>
-  <colItems count="10">
-    <i>
-      <x v="2"/>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="4"/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="5"/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Run_Time" fld="4" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -20851,8 +20850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF292D99-A09D-FD43-ACCE-5F4507DF9B9E}">
   <dimension ref="A1:BG1288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="75" workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q33:T33"/>
+    <sheetView tabSelected="1" topLeftCell="N21" zoomScale="75" workbookViewId="0">
+      <selection activeCell="R48" sqref="R48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21249,94 +21248,91 @@
       <c r="Q5" s="3">
         <v>10</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5">
         <v>6.467804002761838</v>
       </c>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5">
+      <c r="T5">
         <v>18.809646314165203</v>
       </c>
-      <c r="U5" s="5">
+      <c r="U5">
         <v>5.7602055757616926</v>
       </c>
-      <c r="V5" s="5">
+      <c r="V5">
         <v>2.9246370287301606</v>
       </c>
-      <c r="W5" s="5">
+      <c r="W5">
         <v>0.69418358771751276</v>
       </c>
-      <c r="X5" s="5">
+      <c r="X5">
         <v>36.033726385639319</v>
       </c>
-      <c r="Y5" s="5">
+      <c r="Y5">
         <v>12.159697466498844</v>
       </c>
-      <c r="Z5" s="5">
+      <c r="Z5">
         <v>4.9492133130940248</v>
       </c>
-      <c r="AA5" s="5">
+      <c r="AA5">
         <v>2.146502176672215</v>
       </c>
       <c r="AG5" s="3">
         <v>10</v>
       </c>
-      <c r="AH5" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI5" s="5"/>
-      <c r="AJ5" s="5">
-        <v>1</v>
-      </c>
-      <c r="AK5" s="5">
-        <v>1</v>
-      </c>
-      <c r="AL5" s="5">
-        <v>1</v>
-      </c>
-      <c r="AM5" s="5">
-        <v>1</v>
-      </c>
-      <c r="AN5" s="5">
-        <v>1</v>
-      </c>
-      <c r="AO5" s="5">
-        <v>1</v>
-      </c>
-      <c r="AP5" s="5">
-        <v>1</v>
-      </c>
-      <c r="AQ5" s="5">
+      <c r="AH5">
+        <v>1</v>
+      </c>
+      <c r="AJ5">
+        <v>1</v>
+      </c>
+      <c r="AK5">
+        <v>1</v>
+      </c>
+      <c r="AL5">
+        <v>1</v>
+      </c>
+      <c r="AM5">
+        <v>1</v>
+      </c>
+      <c r="AN5">
+        <v>1</v>
+      </c>
+      <c r="AO5">
+        <v>1</v>
+      </c>
+      <c r="AP5">
+        <v>1</v>
+      </c>
+      <c r="AQ5">
         <v>1</v>
       </c>
       <c r="AW5" s="3">
         <v>10</v>
       </c>
-      <c r="AX5" s="5">
+      <c r="AX5">
         <v>0.17616000000000001</v>
       </c>
-      <c r="AY5" s="5"/>
-      <c r="AZ5" s="5">
+      <c r="AZ5">
         <v>4.4880000000000003E-2</v>
       </c>
-      <c r="BA5" s="5">
+      <c r="BA5">
         <v>2.8733333333333329E-2</v>
       </c>
-      <c r="BB5" s="5">
+      <c r="BB5">
         <v>4.4833333333333329E-2</v>
       </c>
-      <c r="BC5" s="5">
+      <c r="BC5">
         <v>7.8780000000000003E-2</v>
       </c>
-      <c r="BD5" s="5">
+      <c r="BD5">
         <v>4.3386666666666657E-2</v>
       </c>
-      <c r="BE5" s="5">
+      <c r="BE5">
         <v>3.8653333333333338E-2</v>
       </c>
-      <c r="BF5" s="5">
+      <c r="BF5">
         <v>3.6540000000000003E-2</v>
       </c>
-      <c r="BG5" s="5">
+      <c r="BG5">
         <v>7.6160000000000005E-2</v>
       </c>
     </row>
@@ -21383,94 +21379,91 @@
       <c r="Q6" s="3">
         <v>20</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R6">
         <v>1418.3588321685763</v>
       </c>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5">
+      <c r="T6">
         <v>49.862430306772325</v>
       </c>
-      <c r="U6" s="5">
+      <c r="U6">
         <v>10.111872560655051</v>
       </c>
-      <c r="V6" s="5">
+      <c r="V6">
         <v>5.2134028061344724</v>
       </c>
-      <c r="W6" s="5">
+      <c r="W6">
         <v>1.3901177113099628</v>
       </c>
-      <c r="X6" s="5">
+      <c r="X6">
         <v>42.342527393127433</v>
       </c>
-      <c r="Y6" s="5">
+      <c r="Y6">
         <v>15.225161170990473</v>
       </c>
-      <c r="Z6" s="5">
+      <c r="Z6">
         <v>7.0602391576704768</v>
       </c>
-      <c r="AA6" s="5">
+      <c r="AA6">
         <v>3.7019937763611432</v>
       </c>
       <c r="AG6" s="3">
         <v>20</v>
       </c>
-      <c r="AH6" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI6" s="5"/>
-      <c r="AJ6" s="5">
-        <v>1</v>
-      </c>
-      <c r="AK6" s="5">
-        <v>1</v>
-      </c>
-      <c r="AL6" s="5">
-        <v>1</v>
-      </c>
-      <c r="AM6" s="5">
-        <v>1</v>
-      </c>
-      <c r="AN6" s="5">
-        <v>1</v>
-      </c>
-      <c r="AO6" s="5">
-        <v>1</v>
-      </c>
-      <c r="AP6" s="5">
-        <v>1</v>
-      </c>
-      <c r="AQ6" s="5">
+      <c r="AH6">
+        <v>1</v>
+      </c>
+      <c r="AJ6">
+        <v>1</v>
+      </c>
+      <c r="AK6">
+        <v>1</v>
+      </c>
+      <c r="AL6">
+        <v>1</v>
+      </c>
+      <c r="AM6">
+        <v>1</v>
+      </c>
+      <c r="AN6">
+        <v>1</v>
+      </c>
+      <c r="AO6">
+        <v>1</v>
+      </c>
+      <c r="AP6">
+        <v>1</v>
+      </c>
+      <c r="AQ6">
         <v>1</v>
       </c>
       <c r="AW6" s="3">
         <v>20</v>
       </c>
-      <c r="AX6" s="5">
+      <c r="AX6">
         <v>0.26444000000000001</v>
       </c>
-      <c r="AY6" s="5"/>
-      <c r="AZ6" s="5">
+      <c r="AZ6">
         <v>6.9955555555555562E-2</v>
       </c>
-      <c r="BA6" s="5">
+      <c r="BA6">
         <v>5.0655555555555565E-2</v>
       </c>
-      <c r="BB6" s="5">
+      <c r="BB6">
         <v>6.647222222222221E-2</v>
       </c>
-      <c r="BC6" s="5">
+      <c r="BC6">
         <v>9.3249999999999986E-2</v>
       </c>
-      <c r="BD6" s="5">
+      <c r="BD6">
         <v>5.6540000000000007E-2</v>
       </c>
-      <c r="BE6" s="5">
+      <c r="BE6">
         <v>5.5113333333333334E-2</v>
       </c>
-      <c r="BF6" s="5">
+      <c r="BF6">
         <v>5.7686666666666671E-2</v>
       </c>
-      <c r="BG6" s="5">
+      <c r="BG6">
         <v>9.9573333333333319E-2</v>
       </c>
     </row>
@@ -21517,94 +21510,91 @@
       <c r="Q7" s="3">
         <v>30</v>
       </c>
-      <c r="R7" s="5">
+      <c r="R7">
         <v>1803.1279098192783</v>
       </c>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5">
+      <c r="T7">
         <v>44.886403556726854</v>
       </c>
-      <c r="U7" s="5">
+      <c r="U7">
         <v>10.823201652305805</v>
       </c>
-      <c r="V7" s="5">
+      <c r="V7">
         <v>5.9025207774092685</v>
       </c>
-      <c r="W7" s="5">
+      <c r="W7">
         <v>2.6656503643530058</v>
       </c>
-      <c r="X7" s="5">
+      <c r="X7">
         <v>51.362631888563392</v>
       </c>
-      <c r="Y7" s="5">
+      <c r="Y7">
         <v>17.516019006849522</v>
       </c>
-      <c r="Z7" s="5">
+      <c r="Z7">
         <v>11.520213649266681</v>
       </c>
-      <c r="AA7" s="5">
+      <c r="AA7">
         <v>5.2616140022252962</v>
       </c>
       <c r="AG7" s="3">
         <v>30</v>
       </c>
-      <c r="AH7" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI7" s="5"/>
-      <c r="AJ7" s="5">
-        <v>1</v>
-      </c>
-      <c r="AK7" s="5">
-        <v>1</v>
-      </c>
-      <c r="AL7" s="5">
-        <v>1</v>
-      </c>
-      <c r="AM7" s="5">
-        <v>1</v>
-      </c>
-      <c r="AN7" s="5">
-        <v>1</v>
-      </c>
-      <c r="AO7" s="5">
-        <v>1</v>
-      </c>
-      <c r="AP7" s="5">
-        <v>1</v>
-      </c>
-      <c r="AQ7" s="5">
+      <c r="AH7">
+        <v>1</v>
+      </c>
+      <c r="AJ7">
+        <v>1</v>
+      </c>
+      <c r="AK7">
+        <v>1</v>
+      </c>
+      <c r="AL7">
+        <v>1</v>
+      </c>
+      <c r="AM7">
+        <v>1</v>
+      </c>
+      <c r="AN7">
+        <v>1</v>
+      </c>
+      <c r="AO7">
+        <v>1</v>
+      </c>
+      <c r="AP7">
+        <v>1</v>
+      </c>
+      <c r="AQ7">
         <v>1</v>
       </c>
       <c r="AW7" s="3">
         <v>30</v>
       </c>
-      <c r="AX7" s="5">
+      <c r="AX7">
         <v>0.35186666666666672</v>
       </c>
-      <c r="AY7" s="5"/>
-      <c r="AZ7" s="5">
+      <c r="AZ7">
         <v>0.11443333333333335</v>
       </c>
-      <c r="BA7" s="5">
+      <c r="BA7">
         <v>8.9406666666666676E-2</v>
       </c>
-      <c r="BB7" s="5">
+      <c r="BB7">
         <v>9.7633333333333322E-2</v>
       </c>
-      <c r="BC7" s="5">
+      <c r="BC7">
         <v>0.10714</v>
       </c>
-      <c r="BD7" s="5">
+      <c r="BD7">
         <v>8.7546666666666662E-2</v>
       </c>
-      <c r="BE7" s="5">
+      <c r="BE7">
         <v>8.7433333333333335E-2</v>
       </c>
-      <c r="BF7" s="5">
+      <c r="BF7">
         <v>9.5960000000000004E-2</v>
       </c>
-      <c r="BG7" s="5">
+      <c r="BG7">
         <v>0.12904000000000002</v>
       </c>
     </row>
@@ -21651,94 +21641,91 @@
       <c r="Q8" s="3">
         <v>40</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8">
         <v>1804.7170451482082</v>
       </c>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5">
+      <c r="T8">
         <v>56.977609445961754</v>
       </c>
-      <c r="U8" s="5">
+      <c r="U8">
         <v>13.528465215116714</v>
       </c>
-      <c r="V8" s="5">
+      <c r="V8">
         <v>7.2305246627889455</v>
       </c>
-      <c r="W8" s="5">
+      <c r="W8">
         <v>2.1324279565364082</v>
       </c>
-      <c r="X8" s="5">
+      <c r="X8">
         <v>58.166022505642125</v>
       </c>
-      <c r="Y8" s="5">
+      <c r="Y8">
         <v>20.15218763329705</v>
       </c>
-      <c r="Z8" s="5">
+      <c r="Z8">
         <v>12.75013032589726</v>
       </c>
-      <c r="AA8" s="5">
+      <c r="AA8">
         <v>7.078381909833583</v>
       </c>
       <c r="AG8" s="3">
         <v>40</v>
       </c>
-      <c r="AH8" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI8" s="5"/>
-      <c r="AJ8" s="5">
-        <v>1</v>
-      </c>
-      <c r="AK8" s="5">
-        <v>1</v>
-      </c>
-      <c r="AL8" s="5">
-        <v>1</v>
-      </c>
-      <c r="AM8" s="5">
-        <v>1</v>
-      </c>
-      <c r="AN8" s="5">
-        <v>1</v>
-      </c>
-      <c r="AO8" s="5">
-        <v>1</v>
-      </c>
-      <c r="AP8" s="5">
-        <v>1</v>
-      </c>
-      <c r="AQ8" s="5">
+      <c r="AH8">
+        <v>1</v>
+      </c>
+      <c r="AJ8">
+        <v>1</v>
+      </c>
+      <c r="AK8">
+        <v>1</v>
+      </c>
+      <c r="AL8">
+        <v>1</v>
+      </c>
+      <c r="AM8">
+        <v>1</v>
+      </c>
+      <c r="AN8">
+        <v>1</v>
+      </c>
+      <c r="AO8">
+        <v>1</v>
+      </c>
+      <c r="AP8">
+        <v>1</v>
+      </c>
+      <c r="AQ8">
         <v>1</v>
       </c>
       <c r="AW8" s="3">
         <v>40</v>
       </c>
-      <c r="AX8" s="5">
+      <c r="AX8">
         <v>0.39575000000000005</v>
       </c>
-      <c r="AY8" s="5"/>
-      <c r="AZ8" s="5">
+      <c r="AZ8">
         <v>0.14077999999999999</v>
       </c>
-      <c r="BA8" s="5">
+      <c r="BA8">
         <v>0.11292666666666666</v>
       </c>
-      <c r="BB8" s="5">
+      <c r="BB8">
         <v>0.13739333333333334</v>
       </c>
-      <c r="BC8" s="5">
+      <c r="BC8">
         <v>0.14391999999999999</v>
       </c>
-      <c r="BD8" s="5">
+      <c r="BD8">
         <v>0.12573999999999999</v>
       </c>
-      <c r="BE8" s="5">
+      <c r="BE8">
         <v>0.10750666666666665</v>
       </c>
-      <c r="BF8" s="5">
+      <c r="BF8">
         <v>0.11045333333333333</v>
       </c>
-      <c r="BG8" s="5">
+      <c r="BG8">
         <v>0.1427066666666667</v>
       </c>
     </row>
@@ -21785,94 +21772,91 @@
       <c r="Q9" s="3">
         <v>50</v>
       </c>
-      <c r="R9" s="5">
+      <c r="R9">
         <v>1805.6749108791312</v>
       </c>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5">
+      <c r="T9">
         <v>36.451838873295671</v>
       </c>
-      <c r="U9" s="5">
+      <c r="U9">
         <v>11.384844934226292</v>
       </c>
-      <c r="V9" s="5">
+      <c r="V9">
         <v>6.2301851922646128</v>
       </c>
-      <c r="W9" s="5">
+      <c r="W9">
         <v>3.1919554679964945</v>
       </c>
-      <c r="X9" s="5">
+      <c r="X9">
         <v>65.588076189346339</v>
       </c>
-      <c r="Y9" s="5">
+      <c r="Y9">
         <v>22.008507391872467</v>
       </c>
-      <c r="Z9" s="5">
+      <c r="Z9">
         <v>14.511934273472628</v>
       </c>
-      <c r="AA9" s="5">
+      <c r="AA9">
         <v>8.3325210780836514</v>
       </c>
       <c r="AG9" s="3">
         <v>50</v>
       </c>
-      <c r="AH9" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI9" s="5"/>
-      <c r="AJ9" s="5">
-        <v>1</v>
-      </c>
-      <c r="AK9" s="5">
-        <v>1</v>
-      </c>
-      <c r="AL9" s="5">
-        <v>1</v>
-      </c>
-      <c r="AM9" s="5">
-        <v>1</v>
-      </c>
-      <c r="AN9" s="5">
-        <v>1</v>
-      </c>
-      <c r="AO9" s="5">
-        <v>1</v>
-      </c>
-      <c r="AP9" s="5">
-        <v>1</v>
-      </c>
-      <c r="AQ9" s="5">
+      <c r="AH9">
+        <v>1</v>
+      </c>
+      <c r="AJ9">
+        <v>1</v>
+      </c>
+      <c r="AK9">
+        <v>1</v>
+      </c>
+      <c r="AL9">
+        <v>1</v>
+      </c>
+      <c r="AM9">
+        <v>1</v>
+      </c>
+      <c r="AN9">
+        <v>1</v>
+      </c>
+      <c r="AO9">
+        <v>1</v>
+      </c>
+      <c r="AP9">
+        <v>1</v>
+      </c>
+      <c r="AQ9">
         <v>1</v>
       </c>
       <c r="AW9" s="3">
         <v>50</v>
       </c>
-      <c r="AX9" s="5">
+      <c r="AX9">
         <v>0.44114000000000003</v>
       </c>
-      <c r="AY9" s="5"/>
-      <c r="AZ9" s="5">
+      <c r="AZ9">
         <v>0.13605999999999999</v>
       </c>
-      <c r="BA9" s="5">
+      <c r="BA9">
         <v>0.11533333333333334</v>
       </c>
-      <c r="BB9" s="5">
+      <c r="BB9">
         <v>0.12112000000000002</v>
       </c>
-      <c r="BC9" s="5">
+      <c r="BC9">
         <v>0.15242000000000003</v>
       </c>
-      <c r="BD9" s="5">
+      <c r="BD9">
         <v>0.14755333333333331</v>
       </c>
-      <c r="BE9" s="5">
+      <c r="BE9">
         <v>0.13538666666666668</v>
       </c>
-      <c r="BF9" s="5">
+      <c r="BF9">
         <v>0.12662000000000001</v>
       </c>
-      <c r="BG9" s="5">
+      <c r="BG9">
         <v>0.16200666666666666</v>
       </c>
     </row>
@@ -21919,94 +21903,91 @@
       <c r="Q10" s="3">
         <v>60</v>
       </c>
-      <c r="R10" s="5">
+      <c r="R10">
         <v>1804.8047039508765</v>
       </c>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5">
+      <c r="T10">
         <v>77.775308542822671</v>
       </c>
-      <c r="U10" s="5">
+      <c r="U10">
         <v>18.063364468980538</v>
       </c>
-      <c r="V10" s="5">
+      <c r="V10">
         <v>10.51072974251581</v>
       </c>
-      <c r="W10" s="5">
+      <c r="W10">
         <v>5.3678272787170931</v>
       </c>
-      <c r="X10" s="5">
+      <c r="X10">
         <v>71.272396031860154</v>
       </c>
-      <c r="Y10" s="5">
+      <c r="Y10">
         <v>25.375562103247837</v>
       </c>
-      <c r="Z10" s="5">
+      <c r="Z10">
         <v>16.535107068003413</v>
       </c>
-      <c r="AA10" s="5">
+      <c r="AA10">
         <v>9.4726466358018193</v>
       </c>
       <c r="AG10" s="3">
         <v>60</v>
       </c>
-      <c r="AH10" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI10" s="5"/>
-      <c r="AJ10" s="5">
-        <v>1</v>
-      </c>
-      <c r="AK10" s="5">
-        <v>1</v>
-      </c>
-      <c r="AL10" s="5">
-        <v>1</v>
-      </c>
-      <c r="AM10" s="5">
-        <v>1</v>
-      </c>
-      <c r="AN10" s="5">
-        <v>1</v>
-      </c>
-      <c r="AO10" s="5">
-        <v>1</v>
-      </c>
-      <c r="AP10" s="5">
-        <v>1</v>
-      </c>
-      <c r="AQ10" s="5">
+      <c r="AH10">
+        <v>1</v>
+      </c>
+      <c r="AJ10">
+        <v>1</v>
+      </c>
+      <c r="AK10">
+        <v>1</v>
+      </c>
+      <c r="AL10">
+        <v>1</v>
+      </c>
+      <c r="AM10">
+        <v>1</v>
+      </c>
+      <c r="AN10">
+        <v>1</v>
+      </c>
+      <c r="AO10">
+        <v>1</v>
+      </c>
+      <c r="AP10">
+        <v>1</v>
+      </c>
+      <c r="AQ10">
         <v>1</v>
       </c>
       <c r="AW10" s="3">
         <v>60</v>
       </c>
-      <c r="AX10" s="5">
+      <c r="AX10">
         <v>0.44661666666666666</v>
       </c>
-      <c r="AY10" s="5"/>
-      <c r="AZ10" s="5">
+      <c r="AZ10">
         <v>0.18319999999999997</v>
       </c>
-      <c r="BA10" s="5">
+      <c r="BA10">
         <v>0.16022</v>
       </c>
-      <c r="BB10" s="5">
+      <c r="BB10">
         <v>0.15468666666666664</v>
       </c>
-      <c r="BC10" s="5">
+      <c r="BC10">
         <v>0.16739333333333334</v>
       </c>
-      <c r="BD10" s="5">
+      <c r="BD10">
         <v>0.17014666666666664</v>
       </c>
-      <c r="BE10" s="5">
+      <c r="BE10">
         <v>0.14961999999999998</v>
       </c>
-      <c r="BF10" s="5">
+      <c r="BF10">
         <v>0.14966666666666664</v>
       </c>
-      <c r="BG10" s="5">
+      <c r="BG10">
         <v>0.17585333333333333</v>
       </c>
     </row>
@@ -22053,94 +22034,91 @@
       <c r="Q11" s="3">
         <v>70</v>
       </c>
-      <c r="R11" s="5">
+      <c r="R11">
         <v>1805.0513837337437</v>
       </c>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5">
+      <c r="T11">
         <v>102.53438437661751</v>
       </c>
-      <c r="U11" s="5">
+      <c r="U11">
         <v>20.153467598929943</v>
       </c>
-      <c r="V11" s="5">
+      <c r="V11">
         <v>11.09627082943914</v>
       </c>
-      <c r="W11" s="5">
+      <c r="W11">
         <v>5.7737360013648731</v>
       </c>
-      <c r="X11" s="5">
+      <c r="X11">
         <v>84.354808643615286</v>
       </c>
-      <c r="Y11" s="5">
+      <c r="Y11">
         <v>27.795951539805735</v>
       </c>
-      <c r="Z11" s="5">
+      <c r="Z11">
         <v>16.24517929994806</v>
       </c>
-      <c r="AA11" s="5">
+      <c r="AA11">
         <v>13.037357867726396</v>
       </c>
       <c r="AG11" s="3">
         <v>70</v>
       </c>
-      <c r="AH11" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI11" s="5"/>
-      <c r="AJ11" s="5">
-        <v>1</v>
-      </c>
-      <c r="AK11" s="5">
-        <v>1</v>
-      </c>
-      <c r="AL11" s="5">
-        <v>1</v>
-      </c>
-      <c r="AM11" s="5">
-        <v>1</v>
-      </c>
-      <c r="AN11" s="5">
-        <v>1</v>
-      </c>
-      <c r="AO11" s="5">
-        <v>1</v>
-      </c>
-      <c r="AP11" s="5">
-        <v>1</v>
-      </c>
-      <c r="AQ11" s="5">
+      <c r="AH11">
+        <v>1</v>
+      </c>
+      <c r="AJ11">
+        <v>1</v>
+      </c>
+      <c r="AK11">
+        <v>1</v>
+      </c>
+      <c r="AL11">
+        <v>1</v>
+      </c>
+      <c r="AM11">
+        <v>1</v>
+      </c>
+      <c r="AN11">
+        <v>1</v>
+      </c>
+      <c r="AO11">
+        <v>1</v>
+      </c>
+      <c r="AP11">
+        <v>1</v>
+      </c>
+      <c r="AQ11">
         <v>1</v>
       </c>
       <c r="AW11" s="3">
         <v>70</v>
       </c>
-      <c r="AX11" s="5">
+      <c r="AX11">
         <v>0.47475000000000001</v>
       </c>
-      <c r="AY11" s="5"/>
-      <c r="AZ11" s="5">
+      <c r="AZ11">
         <v>0.20323333333333332</v>
       </c>
-      <c r="BA11" s="5">
+      <c r="BA11">
         <v>0.17903333333333332</v>
       </c>
-      <c r="BB11" s="5">
+      <c r="BB11">
         <v>0.15969333333333335</v>
       </c>
-      <c r="BC11" s="5">
+      <c r="BC11">
         <v>0.19869333333333333</v>
       </c>
-      <c r="BD11" s="5">
+      <c r="BD11">
         <v>0.18173999999999998</v>
       </c>
-      <c r="BE11" s="5">
+      <c r="BE11">
         <v>0.16350000000000001</v>
       </c>
-      <c r="BF11" s="5">
+      <c r="BF11">
         <v>0.17335999999999999</v>
       </c>
-      <c r="BG11" s="5">
+      <c r="BG11">
         <v>0.19428666666666669</v>
       </c>
     </row>
@@ -22187,94 +22165,91 @@
       <c r="Q12" s="3">
         <v>80</v>
       </c>
-      <c r="R12" s="5">
+      <c r="R12">
         <v>1806.07922816276</v>
       </c>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5">
+      <c r="T12">
         <v>85.926192390305459</v>
       </c>
-      <c r="U12" s="5">
+      <c r="U12">
         <v>26.185760986641935</v>
       </c>
-      <c r="V12" s="5">
+      <c r="V12">
         <v>14.40519138646774</v>
       </c>
-      <c r="W12" s="5">
+      <c r="W12">
         <v>7.4039643921035614</v>
       </c>
-      <c r="X12" s="5">
+      <c r="X12">
         <v>87.127395424929531</v>
       </c>
-      <c r="Y12" s="5">
+      <c r="Y12">
         <v>26.195546935809102</v>
       </c>
-      <c r="Z12" s="5">
+      <c r="Z12">
         <v>20.470129467081218</v>
       </c>
-      <c r="AA12" s="5">
+      <c r="AA12">
         <v>12.751489553973022</v>
       </c>
       <c r="AG12" s="3">
         <v>80</v>
       </c>
-      <c r="AH12" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI12" s="5"/>
-      <c r="AJ12" s="5">
-        <v>1</v>
-      </c>
-      <c r="AK12" s="5">
-        <v>1</v>
-      </c>
-      <c r="AL12" s="5">
-        <v>1</v>
-      </c>
-      <c r="AM12" s="5">
-        <v>1</v>
-      </c>
-      <c r="AN12" s="5">
-        <v>1</v>
-      </c>
-      <c r="AO12" s="5">
-        <v>1</v>
-      </c>
-      <c r="AP12" s="5">
-        <v>1</v>
-      </c>
-      <c r="AQ12" s="5">
+      <c r="AH12">
+        <v>1</v>
+      </c>
+      <c r="AJ12">
+        <v>1</v>
+      </c>
+      <c r="AK12">
+        <v>1</v>
+      </c>
+      <c r="AL12">
+        <v>1</v>
+      </c>
+      <c r="AM12">
+        <v>1</v>
+      </c>
+      <c r="AN12">
+        <v>1</v>
+      </c>
+      <c r="AO12">
+        <v>1</v>
+      </c>
+      <c r="AP12">
+        <v>1</v>
+      </c>
+      <c r="AQ12">
         <v>1</v>
       </c>
       <c r="AW12" s="3">
         <v>80</v>
       </c>
-      <c r="AX12" s="5">
+      <c r="AX12">
         <v>0.48336000000000007</v>
       </c>
-      <c r="AY12" s="5"/>
-      <c r="AZ12" s="5">
+      <c r="AZ12">
         <v>0.19779166666666667</v>
       </c>
-      <c r="BA12" s="5">
+      <c r="BA12">
         <v>0.17874166666666666</v>
       </c>
-      <c r="BB12" s="5">
+      <c r="BB12">
         <v>0.18084166666666668</v>
       </c>
-      <c r="BC12" s="5">
+      <c r="BC12">
         <v>0.21479166666666669</v>
       </c>
-      <c r="BD12" s="5">
+      <c r="BD12">
         <v>0.20536666666666667</v>
       </c>
-      <c r="BE12" s="5">
+      <c r="BE12">
         <v>0.19451333333333334</v>
       </c>
-      <c r="BF12" s="5">
+      <c r="BF12">
         <v>0.1796733333333333</v>
       </c>
-      <c r="BG12" s="5">
+      <c r="BG12">
         <v>0.2147</v>
       </c>
     </row>
@@ -22321,94 +22296,91 @@
       <c r="Q13" s="3">
         <v>90</v>
       </c>
-      <c r="R13" s="5">
+      <c r="R13">
         <v>1804.6172080039917</v>
       </c>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5">
+      <c r="T13">
         <v>109.7498666395431</v>
       </c>
-      <c r="U13" s="5">
+      <c r="U13">
         <v>25.047420697969653</v>
       </c>
-      <c r="V13" s="5">
+      <c r="V13">
         <v>15.454676831234211</v>
       </c>
-      <c r="W13" s="5">
+      <c r="W13">
         <v>6.9276429510675195</v>
       </c>
-      <c r="X13" s="5">
+      <c r="X13">
         <v>92.171983112860332</v>
       </c>
-      <c r="Y13" s="5">
+      <c r="Y13">
         <v>31.724773276690353</v>
       </c>
-      <c r="Z13" s="5">
+      <c r="Z13">
         <v>21.319558002923877</v>
       </c>
-      <c r="AA13" s="5">
+      <c r="AA13">
         <v>15.044225171705033</v>
       </c>
       <c r="AG13" s="3">
         <v>90</v>
       </c>
-      <c r="AH13" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI13" s="5"/>
-      <c r="AJ13" s="5">
-        <v>1</v>
-      </c>
-      <c r="AK13" s="5">
-        <v>1</v>
-      </c>
-      <c r="AL13" s="5">
-        <v>1</v>
-      </c>
-      <c r="AM13" s="5">
-        <v>1</v>
-      </c>
-      <c r="AN13" s="5">
-        <v>1</v>
-      </c>
-      <c r="AO13" s="5">
-        <v>1</v>
-      </c>
-      <c r="AP13" s="5">
-        <v>1</v>
-      </c>
-      <c r="AQ13" s="5">
+      <c r="AH13">
+        <v>1</v>
+      </c>
+      <c r="AJ13">
+        <v>1</v>
+      </c>
+      <c r="AK13">
+        <v>1</v>
+      </c>
+      <c r="AL13">
+        <v>1</v>
+      </c>
+      <c r="AM13">
+        <v>1</v>
+      </c>
+      <c r="AN13">
+        <v>1</v>
+      </c>
+      <c r="AO13">
+        <v>1</v>
+      </c>
+      <c r="AP13">
+        <v>1</v>
+      </c>
+      <c r="AQ13">
         <v>1</v>
       </c>
       <c r="AW13" s="3">
         <v>90</v>
       </c>
-      <c r="AX13" s="5">
+      <c r="AX13">
         <v>0.50861666666666672</v>
       </c>
-      <c r="AY13" s="5"/>
-      <c r="AZ13" s="5">
+      <c r="AZ13">
         <v>0.24461333333333338</v>
       </c>
-      <c r="BA13" s="5">
+      <c r="BA13">
         <v>0.23328666666666673</v>
       </c>
-      <c r="BB13" s="5">
+      <c r="BB13">
         <v>0.2117</v>
       </c>
-      <c r="BC13" s="5">
+      <c r="BC13">
         <v>0.23028666666666667</v>
       </c>
-      <c r="BD13" s="5">
+      <c r="BD13">
         <v>0.22526000000000002</v>
       </c>
-      <c r="BE13" s="5">
+      <c r="BE13">
         <v>0.20520666666666668</v>
       </c>
-      <c r="BF13" s="5">
+      <c r="BF13">
         <v>0.20017333333333331</v>
       </c>
-      <c r="BG13" s="5">
+      <c r="BG13">
         <v>0.24383333333333332</v>
       </c>
     </row>
@@ -22455,94 +22427,91 @@
       <c r="Q14" s="3">
         <v>100</v>
       </c>
-      <c r="R14" s="5">
+      <c r="R14">
         <v>1804.5764752387961</v>
       </c>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5">
+      <c r="T14">
         <v>57.43862792194502</v>
       </c>
-      <c r="U14" s="5">
+      <c r="U14">
         <v>14.843114964291408</v>
       </c>
-      <c r="V14" s="5">
+      <c r="V14">
         <v>9.2697486129899609</v>
       </c>
-      <c r="W14" s="5">
+      <c r="W14">
         <v>6.1064946904157562</v>
       </c>
-      <c r="X14" s="5">
+      <c r="X14">
         <v>97.398843279511794</v>
       </c>
-      <c r="Y14" s="5">
+      <c r="Y14">
         <v>33.429966646308671</v>
       </c>
-      <c r="Z14" s="5">
+      <c r="Z14">
         <v>24.145781913182336</v>
       </c>
-      <c r="AA14" s="5">
+      <c r="AA14">
         <v>16.539990947178193</v>
       </c>
       <c r="AG14" s="3">
         <v>100</v>
       </c>
-      <c r="AH14" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI14" s="5"/>
-      <c r="AJ14" s="5">
-        <v>1</v>
-      </c>
-      <c r="AK14" s="5">
-        <v>1</v>
-      </c>
-      <c r="AL14" s="5">
-        <v>1</v>
-      </c>
-      <c r="AM14" s="5">
-        <v>1</v>
-      </c>
-      <c r="AN14" s="5">
-        <v>1</v>
-      </c>
-      <c r="AO14" s="5">
-        <v>1</v>
-      </c>
-      <c r="AP14" s="5">
-        <v>1</v>
-      </c>
-      <c r="AQ14" s="5">
+      <c r="AH14">
+        <v>1</v>
+      </c>
+      <c r="AJ14">
+        <v>1</v>
+      </c>
+      <c r="AK14">
+        <v>1</v>
+      </c>
+      <c r="AL14">
+        <v>1</v>
+      </c>
+      <c r="AM14">
+        <v>1</v>
+      </c>
+      <c r="AN14">
+        <v>1</v>
+      </c>
+      <c r="AO14">
+        <v>1</v>
+      </c>
+      <c r="AP14">
+        <v>1</v>
+      </c>
+      <c r="AQ14">
         <v>1</v>
       </c>
       <c r="AW14" s="3">
         <v>100</v>
       </c>
-      <c r="AX14" s="5">
+      <c r="AX14">
         <v>0.51880000000000004</v>
       </c>
-      <c r="AY14" s="5"/>
-      <c r="AZ14" s="5">
+      <c r="AZ14">
         <v>0.24506000000000003</v>
       </c>
-      <c r="BA14" s="5">
+      <c r="BA14">
         <v>0.23709333333333332</v>
       </c>
-      <c r="BB14" s="5">
+      <c r="BB14">
         <v>0.21558666666666668</v>
       </c>
-      <c r="BC14" s="5">
+      <c r="BC14">
         <v>0.24607333333333334</v>
       </c>
-      <c r="BD14" s="5">
+      <c r="BD14">
         <v>0.25405333333333335</v>
       </c>
-      <c r="BE14" s="5">
+      <c r="BE14">
         <v>0.23025333333333331</v>
       </c>
-      <c r="BF14" s="5">
+      <c r="BF14">
         <v>0.21951333333333334</v>
       </c>
-      <c r="BG14" s="5">
+      <c r="BG14">
         <v>0.24041999999999997</v>
       </c>
     </row>
@@ -22589,42 +22558,12 @@
       <c r="Q15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
-      <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
-      <c r="Y15" s="5"/>
-      <c r="Z15" s="5"/>
-      <c r="AA15" s="5"/>
       <c r="AG15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AH15" s="5"/>
-      <c r="AI15" s="5"/>
-      <c r="AJ15" s="5"/>
-      <c r="AK15" s="5"/>
-      <c r="AL15" s="5"/>
-      <c r="AM15" s="5"/>
-      <c r="AN15" s="5"/>
-      <c r="AO15" s="5"/>
-      <c r="AP15" s="5"/>
-      <c r="AQ15" s="5"/>
       <c r="AW15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AX15" s="5"/>
-      <c r="AY15" s="5"/>
-      <c r="AZ15" s="5"/>
-      <c r="BA15" s="5"/>
-      <c r="BB15" s="5"/>
-      <c r="BC15" s="5"/>
-      <c r="BD15" s="5"/>
-      <c r="BE15" s="5"/>
-      <c r="BF15" s="5"/>
-      <c r="BG15" s="5"/>
     </row>
     <row r="16" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -23027,48 +22966,21 @@
       <c r="Q21" s="3">
         <v>10</v>
       </c>
-      <c r="R21" s="5">
+      <c r="R21">
         <v>98560.393400929403</v>
       </c>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
-      <c r="V21" s="5"/>
-      <c r="W21" s="5"/>
-      <c r="X21" s="5"/>
-      <c r="Y21" s="5"/>
-      <c r="Z21" s="5"/>
-      <c r="AA21" s="5"/>
       <c r="AG21" s="3">
         <v>10</v>
       </c>
-      <c r="AH21" s="5">
+      <c r="AH21">
         <v>98567.315808344138</v>
       </c>
-      <c r="AI21" s="5"/>
-      <c r="AJ21" s="5"/>
-      <c r="AK21" s="5"/>
-      <c r="AL21" s="5"/>
-      <c r="AM21" s="5"/>
-      <c r="AN21" s="5"/>
-      <c r="AO21" s="5"/>
-      <c r="AP21" s="5"/>
-      <c r="AQ21" s="5"/>
       <c r="AW21" s="3">
         <v>10</v>
       </c>
-      <c r="AX21" s="5">
+      <c r="AX21">
         <v>6.8872769552687701E-5</v>
       </c>
-      <c r="AY21" s="5"/>
-      <c r="AZ21" s="5"/>
-      <c r="BA21" s="5"/>
-      <c r="BB21" s="5"/>
-      <c r="BC21" s="5"/>
-      <c r="BD21" s="5"/>
-      <c r="BE21" s="5"/>
-      <c r="BF21" s="5"/>
-      <c r="BG21" s="5"/>
     </row>
     <row r="22" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A22">
@@ -23113,48 +23025,21 @@
       <c r="Q22" s="3">
         <v>20</v>
       </c>
-      <c r="R22" s="5">
+      <c r="R22">
         <v>78770.19351097921</v>
       </c>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
-      <c r="V22" s="5"/>
-      <c r="W22" s="5"/>
-      <c r="X22" s="5"/>
-      <c r="Y22" s="5"/>
-      <c r="Z22" s="5"/>
-      <c r="AA22" s="5"/>
       <c r="AG22" s="3">
         <v>20</v>
       </c>
-      <c r="AH22" s="5">
+      <c r="AH22">
         <v>78782.99243727143</v>
       </c>
-      <c r="AI22" s="5"/>
-      <c r="AJ22" s="5"/>
-      <c r="AK22" s="5"/>
-      <c r="AL22" s="5"/>
-      <c r="AM22" s="5"/>
-      <c r="AN22" s="5"/>
-      <c r="AO22" s="5"/>
-      <c r="AP22" s="5"/>
-      <c r="AQ22" s="5"/>
       <c r="AW22" s="3">
         <v>20</v>
       </c>
-      <c r="AX22" s="5">
+      <c r="AX22">
         <v>1.6457748190060607E-4</v>
       </c>
-      <c r="AY22" s="5"/>
-      <c r="AZ22" s="5"/>
-      <c r="BA22" s="5"/>
-      <c r="BB22" s="5"/>
-      <c r="BC22" s="5"/>
-      <c r="BD22" s="5"/>
-      <c r="BE22" s="5"/>
-      <c r="BF22" s="5"/>
-      <c r="BG22" s="5"/>
     </row>
     <row r="23" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A23">
@@ -23199,48 +23084,21 @@
       <c r="Q23" s="3">
         <v>30</v>
       </c>
-      <c r="R23" s="5">
+      <c r="R23">
         <v>65457.662359005219</v>
       </c>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
-      <c r="U23" s="5"/>
-      <c r="V23" s="5"/>
-      <c r="W23" s="5"/>
-      <c r="X23" s="5"/>
-      <c r="Y23" s="5"/>
-      <c r="Z23" s="5"/>
-      <c r="AA23" s="5"/>
       <c r="AG23" s="3">
         <v>30</v>
       </c>
-      <c r="AH23" s="5">
+      <c r="AH23">
         <v>65554.357525763102</v>
       </c>
-      <c r="AI23" s="5"/>
-      <c r="AJ23" s="5"/>
-      <c r="AK23" s="5"/>
-      <c r="AL23" s="5"/>
-      <c r="AM23" s="5"/>
-      <c r="AN23" s="5"/>
-      <c r="AO23" s="5"/>
-      <c r="AP23" s="5"/>
-      <c r="AQ23" s="5"/>
       <c r="AW23" s="3">
         <v>30</v>
       </c>
-      <c r="AX23" s="5">
+      <c r="AX23">
         <v>1.4821862712955881E-3</v>
       </c>
-      <c r="AY23" s="5"/>
-      <c r="AZ23" s="5"/>
-      <c r="BA23" s="5"/>
-      <c r="BB23" s="5"/>
-      <c r="BC23" s="5"/>
-      <c r="BD23" s="5"/>
-      <c r="BE23" s="5"/>
-      <c r="BF23" s="5"/>
-      <c r="BG23" s="5"/>
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A24">
@@ -23285,48 +23143,21 @@
       <c r="Q24" s="3">
         <v>40</v>
       </c>
-      <c r="R24" s="5">
+      <c r="R24">
         <v>60026.995481943981</v>
       </c>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
-      <c r="V24" s="5"/>
-      <c r="W24" s="5"/>
-      <c r="X24" s="5"/>
-      <c r="Y24" s="5"/>
-      <c r="Z24" s="5"/>
-      <c r="AA24" s="5"/>
       <c r="AG24" s="3">
         <v>40</v>
       </c>
-      <c r="AH24" s="5">
+      <c r="AH24">
         <v>60222.991115606092</v>
       </c>
-      <c r="AI24" s="5"/>
-      <c r="AJ24" s="5"/>
-      <c r="AK24" s="5"/>
-      <c r="AL24" s="5"/>
-      <c r="AM24" s="5"/>
-      <c r="AN24" s="5"/>
-      <c r="AO24" s="5"/>
-      <c r="AP24" s="5"/>
-      <c r="AQ24" s="5"/>
       <c r="AW24" s="3">
         <v>40</v>
       </c>
-      <c r="AX24" s="5">
+      <c r="AX24">
         <v>3.2814473695154879E-3</v>
       </c>
-      <c r="AY24" s="5"/>
-      <c r="AZ24" s="5"/>
-      <c r="BA24" s="5"/>
-      <c r="BB24" s="5"/>
-      <c r="BC24" s="5"/>
-      <c r="BD24" s="5"/>
-      <c r="BE24" s="5"/>
-      <c r="BF24" s="5"/>
-      <c r="BG24" s="5"/>
     </row>
     <row r="25" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A25">
@@ -23371,48 +23202,21 @@
       <c r="Q25" s="3">
         <v>50</v>
       </c>
-      <c r="R25" s="5">
+      <c r="R25">
         <v>55801.796263412616</v>
       </c>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
-      <c r="U25" s="5"/>
-      <c r="V25" s="5"/>
-      <c r="W25" s="5"/>
-      <c r="X25" s="5"/>
-      <c r="Y25" s="5"/>
-      <c r="Z25" s="5"/>
-      <c r="AA25" s="5"/>
       <c r="AG25" s="3">
         <v>50</v>
       </c>
-      <c r="AH25" s="5">
+      <c r="AH25">
         <v>56083.86175776356</v>
       </c>
-      <c r="AI25" s="5"/>
-      <c r="AJ25" s="5"/>
-      <c r="AK25" s="5"/>
-      <c r="AL25" s="5"/>
-      <c r="AM25" s="5"/>
-      <c r="AN25" s="5"/>
-      <c r="AO25" s="5"/>
-      <c r="AP25" s="5"/>
-      <c r="AQ25" s="5"/>
       <c r="AW25" s="3">
         <v>50</v>
       </c>
-      <c r="AX25" s="5">
+      <c r="AX25">
         <v>5.0697162468863683E-3</v>
       </c>
-      <c r="AY25" s="5"/>
-      <c r="AZ25" s="5"/>
-      <c r="BA25" s="5"/>
-      <c r="BB25" s="5"/>
-      <c r="BC25" s="5"/>
-      <c r="BD25" s="5"/>
-      <c r="BE25" s="5"/>
-      <c r="BF25" s="5"/>
-      <c r="BG25" s="5"/>
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A26">
@@ -23457,48 +23261,21 @@
       <c r="Q26" s="3">
         <v>60</v>
       </c>
-      <c r="R26" s="5">
+      <c r="R26">
         <v>51535.327305449006</v>
       </c>
-      <c r="S26" s="5"/>
-      <c r="T26" s="5"/>
-      <c r="U26" s="5"/>
-      <c r="V26" s="5"/>
-      <c r="W26" s="5"/>
-      <c r="X26" s="5"/>
-      <c r="Y26" s="5"/>
-      <c r="Z26" s="5"/>
-      <c r="AA26" s="5"/>
       <c r="AG26" s="3">
         <v>60</v>
       </c>
-      <c r="AH26" s="5">
+      <c r="AH26">
         <v>51904.439115680296</v>
       </c>
-      <c r="AI26" s="5"/>
-      <c r="AJ26" s="5"/>
-      <c r="AK26" s="5"/>
-      <c r="AL26" s="5"/>
-      <c r="AM26" s="5"/>
-      <c r="AN26" s="5"/>
-      <c r="AO26" s="5"/>
-      <c r="AP26" s="5"/>
-      <c r="AQ26" s="5"/>
       <c r="AW26" s="3">
         <v>60</v>
       </c>
-      <c r="AX26" s="5">
+      <c r="AX26">
         <v>7.1826249761124629E-3</v>
       </c>
-      <c r="AY26" s="5"/>
-      <c r="AZ26" s="5"/>
-      <c r="BA26" s="5"/>
-      <c r="BB26" s="5"/>
-      <c r="BC26" s="5"/>
-      <c r="BD26" s="5"/>
-      <c r="BE26" s="5"/>
-      <c r="BF26" s="5"/>
-      <c r="BG26" s="5"/>
     </row>
     <row r="27" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -23543,48 +23320,21 @@
       <c r="Q27" s="3">
         <v>70</v>
       </c>
-      <c r="R27" s="5">
+      <c r="R27">
         <v>48628.162434219739</v>
       </c>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
-      <c r="U27" s="5"/>
-      <c r="V27" s="5"/>
-      <c r="W27" s="5"/>
-      <c r="X27" s="5"/>
-      <c r="Y27" s="5"/>
-      <c r="Z27" s="5"/>
-      <c r="AA27" s="5"/>
       <c r="AG27" s="3">
         <v>70</v>
       </c>
-      <c r="AH27" s="5">
+      <c r="AH27">
         <v>49059.67697716158</v>
       </c>
-      <c r="AI27" s="5"/>
-      <c r="AJ27" s="5"/>
-      <c r="AK27" s="5"/>
-      <c r="AL27" s="5"/>
-      <c r="AM27" s="5"/>
-      <c r="AN27" s="5"/>
-      <c r="AO27" s="5"/>
-      <c r="AP27" s="5"/>
-      <c r="AQ27" s="5"/>
       <c r="AW27" s="3">
         <v>70</v>
       </c>
-      <c r="AX27" s="5">
+      <c r="AX27">
         <v>8.9091674886259079E-3</v>
       </c>
-      <c r="AY27" s="5"/>
-      <c r="AZ27" s="5"/>
-      <c r="BA27" s="5"/>
-      <c r="BB27" s="5"/>
-      <c r="BC27" s="5"/>
-      <c r="BD27" s="5"/>
-      <c r="BE27" s="5"/>
-      <c r="BF27" s="5"/>
-      <c r="BG27" s="5"/>
     </row>
     <row r="28" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A28">
@@ -23629,48 +23379,21 @@
       <c r="Q28" s="3">
         <v>80</v>
       </c>
-      <c r="R28" s="5">
+      <c r="R28">
         <v>46285.595631525575</v>
       </c>
-      <c r="S28" s="5"/>
-      <c r="T28" s="5"/>
-      <c r="U28" s="5"/>
-      <c r="V28" s="5"/>
-      <c r="W28" s="5"/>
-      <c r="X28" s="5"/>
-      <c r="Y28" s="5"/>
-      <c r="Z28" s="5"/>
-      <c r="AA28" s="5"/>
       <c r="AG28" s="3">
         <v>80</v>
       </c>
-      <c r="AH28" s="5">
+      <c r="AH28">
         <v>46729.585759188718</v>
       </c>
-      <c r="AI28" s="5"/>
-      <c r="AJ28" s="5"/>
-      <c r="AK28" s="5"/>
-      <c r="AL28" s="5"/>
-      <c r="AM28" s="5"/>
-      <c r="AN28" s="5"/>
-      <c r="AO28" s="5"/>
-      <c r="AP28" s="5"/>
-      <c r="AQ28" s="5"/>
       <c r="AW28" s="3">
         <v>80</v>
       </c>
-      <c r="AX28" s="5">
+      <c r="AX28">
         <v>9.6103852627402227E-3</v>
       </c>
-      <c r="AY28" s="5"/>
-      <c r="AZ28" s="5"/>
-      <c r="BA28" s="5"/>
-      <c r="BB28" s="5"/>
-      <c r="BC28" s="5"/>
-      <c r="BD28" s="5"/>
-      <c r="BE28" s="5"/>
-      <c r="BF28" s="5"/>
-      <c r="BG28" s="5"/>
     </row>
     <row r="29" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -23715,48 +23438,21 @@
       <c r="Q29" s="3">
         <v>90</v>
       </c>
-      <c r="R29" s="5">
+      <c r="R29">
         <v>43203.162336393936</v>
       </c>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
-      <c r="U29" s="5"/>
-      <c r="V29" s="5"/>
-      <c r="W29" s="5"/>
-      <c r="X29" s="5"/>
-      <c r="Y29" s="5"/>
-      <c r="Z29" s="5"/>
-      <c r="AA29" s="5"/>
       <c r="AG29" s="3">
         <v>90</v>
       </c>
-      <c r="AH29" s="5">
+      <c r="AH29">
         <v>43720.005538765421</v>
       </c>
-      <c r="AI29" s="5"/>
-      <c r="AJ29" s="5"/>
-      <c r="AK29" s="5"/>
-      <c r="AL29" s="5"/>
-      <c r="AM29" s="5"/>
-      <c r="AN29" s="5"/>
-      <c r="AO29" s="5"/>
-      <c r="AP29" s="5"/>
-      <c r="AQ29" s="5"/>
       <c r="AW29" s="3">
         <v>90</v>
       </c>
-      <c r="AX29" s="5">
+      <c r="AX29">
         <v>1.1975478975970252E-2</v>
       </c>
-      <c r="AY29" s="5"/>
-      <c r="AZ29" s="5"/>
-      <c r="BA29" s="5"/>
-      <c r="BB29" s="5"/>
-      <c r="BC29" s="5"/>
-      <c r="BD29" s="5"/>
-      <c r="BE29" s="5"/>
-      <c r="BF29" s="5"/>
-      <c r="BG29" s="5"/>
     </row>
     <row r="30" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -23801,48 +23497,21 @@
       <c r="Q30" s="3">
         <v>100</v>
       </c>
-      <c r="R30" s="5">
+      <c r="R30">
         <v>41014.194202061801</v>
       </c>
-      <c r="S30" s="5"/>
-      <c r="T30" s="5"/>
-      <c r="U30" s="5"/>
-      <c r="V30" s="5"/>
-      <c r="W30" s="5"/>
-      <c r="X30" s="5"/>
-      <c r="Y30" s="5"/>
-      <c r="Z30" s="5"/>
-      <c r="AA30" s="5"/>
       <c r="AG30" s="3">
         <v>100</v>
       </c>
-      <c r="AH30" s="5">
+      <c r="AH30">
         <v>41569.903584112901</v>
       </c>
-      <c r="AI30" s="5"/>
-      <c r="AJ30" s="5"/>
-      <c r="AK30" s="5"/>
-      <c r="AL30" s="5"/>
-      <c r="AM30" s="5"/>
-      <c r="AN30" s="5"/>
-      <c r="AO30" s="5"/>
-      <c r="AP30" s="5"/>
-      <c r="AQ30" s="5"/>
       <c r="AW30" s="3">
         <v>100</v>
       </c>
-      <c r="AX30" s="5">
+      <c r="AX30">
         <v>1.363919884981094E-2</v>
       </c>
-      <c r="AY30" s="5"/>
-      <c r="AZ30" s="5"/>
-      <c r="BA30" s="5"/>
-      <c r="BB30" s="5"/>
-      <c r="BC30" s="5"/>
-      <c r="BD30" s="5"/>
-      <c r="BE30" s="5"/>
-      <c r="BF30" s="5"/>
-      <c r="BG30" s="5"/>
     </row>
     <row r="31" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -23887,42 +23556,12 @@
       <c r="Q31" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
-      <c r="U31" s="5"/>
-      <c r="V31" s="5"/>
-      <c r="W31" s="5"/>
-      <c r="X31" s="5"/>
-      <c r="Y31" s="5"/>
-      <c r="Z31" s="5"/>
-      <c r="AA31" s="5"/>
       <c r="AG31" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AH31" s="5"/>
-      <c r="AI31" s="5"/>
-      <c r="AJ31" s="5"/>
-      <c r="AK31" s="5"/>
-      <c r="AL31" s="5"/>
-      <c r="AM31" s="5"/>
-      <c r="AN31" s="5"/>
-      <c r="AO31" s="5"/>
-      <c r="AP31" s="5"/>
-      <c r="AQ31" s="5"/>
       <c r="AW31" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AX31" s="5"/>
-      <c r="AY31" s="5"/>
-      <c r="AZ31" s="5"/>
-      <c r="BA31" s="5"/>
-      <c r="BB31" s="5"/>
-      <c r="BC31" s="5"/>
-      <c r="BD31" s="5"/>
-      <c r="BE31" s="5"/>
-      <c r="BF31" s="5"/>
-      <c r="BG31" s="5"/>
     </row>
     <row r="32" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -23965,38 +23604,8 @@
         <v>63898.867006243803</v>
       </c>
       <c r="Q32" s="3"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
-      <c r="U32" s="5"/>
-      <c r="V32" s="5"/>
-      <c r="W32" s="5"/>
-      <c r="X32" s="5"/>
-      <c r="Y32" s="5"/>
-      <c r="Z32" s="5"/>
-      <c r="AA32" s="5"/>
       <c r="AG32" s="3"/>
-      <c r="AH32" s="5"/>
-      <c r="AI32" s="5"/>
-      <c r="AJ32" s="5"/>
-      <c r="AK32" s="5"/>
-      <c r="AL32" s="5"/>
-      <c r="AM32" s="5"/>
-      <c r="AN32" s="5"/>
-      <c r="AO32" s="5"/>
-      <c r="AP32" s="5"/>
-      <c r="AQ32" s="5"/>
       <c r="AW32" s="3"/>
-      <c r="AX32" s="5"/>
-      <c r="AY32" s="5"/>
-      <c r="AZ32" s="5"/>
-      <c r="BA32" s="5"/>
-      <c r="BB32" s="5"/>
-      <c r="BC32" s="5"/>
-      <c r="BD32" s="5"/>
-      <c r="BE32" s="5"/>
-      <c r="BF32" s="5"/>
-      <c r="BG32" s="5"/>
     </row>
     <row r="33" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A33">
@@ -24038,12 +23647,12 @@
       <c r="M33">
         <v>64825.985691161201</v>
       </c>
-      <c r="Q33" s="4" t="s">
+      <c r="Q33" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6"/>
+      <c r="T33" s="6"/>
     </row>
     <row r="34" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A34">
@@ -24085,16 +23694,16 @@
       <c r="M34">
         <v>64146.193789065197</v>
       </c>
-      <c r="R34" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="S34" s="4"/>
-      <c r="T34" s="4"/>
-      <c r="U34" s="4" t="s">
+      <c r="R34" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="S34" s="6"/>
+      <c r="T34" s="6"/>
+      <c r="U34" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="V34" s="4"/>
-      <c r="W34" s="4"/>
+      <c r="V34" s="6"/>
+      <c r="W34" s="6"/>
       <c r="AG34" t="s">
         <v>49</v>
       </c>
@@ -24173,7 +23782,7 @@
         <v>0.17616000000000001</v>
       </c>
       <c r="AI35">
-        <f>AVERAGE(BA5:BD5)</f>
+        <f t="shared" ref="AI35:AI44" si="0">AVERAGE(BA5:BD5)</f>
         <v>4.8933333333333329E-2</v>
       </c>
       <c r="AM35" t="s">
@@ -24230,7 +23839,7 @@
       <c r="M36">
         <v>66837.1078170541</v>
       </c>
-      <c r="Q36" s="6">
+      <c r="Q36" s="4">
         <v>10</v>
       </c>
       <c r="R36">
@@ -24245,7 +23854,7 @@
         <v>17.62</v>
       </c>
       <c r="U36">
-        <f>ROUND(AVERAGE(U5:X5),2)</f>
+        <f t="shared" ref="U36:U45" si="1">ROUND(AVERAGE(U5:X5),2)</f>
         <v>11.35</v>
       </c>
       <c r="V36">
@@ -24262,7 +23871,7 @@
         <v>0.26444000000000001</v>
       </c>
       <c r="AI36">
-        <f>AVERAGE(BA6:BD6)</f>
+        <f t="shared" si="0"/>
         <v>6.6729444444444452E-2</v>
       </c>
       <c r="AL36" t="s">
@@ -24322,29 +23931,29 @@
       <c r="M37">
         <v>66780.888338352903</v>
       </c>
-      <c r="Q37" s="6">
+      <c r="Q37" s="4">
         <v>20</v>
       </c>
       <c r="R37">
-        <f t="shared" ref="R37:R45" si="0">ROUND(AG36,2)</f>
+        <f t="shared" ref="R37:R45" si="2">ROUND(AG36,2)</f>
         <v>1418.35</v>
       </c>
       <c r="S37">
         <v>1</v>
       </c>
       <c r="T37">
-        <f t="shared" ref="T37:T45" si="1">ROUND(100*AH36,2)</f>
+        <f t="shared" ref="T37:T45" si="3">ROUND(100*AH36,2)</f>
         <v>26.44</v>
       </c>
       <c r="U37">
-        <f>ROUND(AVERAGE(U6:X6),2)</f>
+        <f t="shared" si="1"/>
         <v>14.76</v>
       </c>
       <c r="V37">
         <v>1</v>
       </c>
       <c r="W37">
-        <f t="shared" ref="W37:W45" si="2">ROUND(100*AI36,2)</f>
+        <f t="shared" ref="W37:W45" si="4">ROUND(100*AI36,2)</f>
         <v>6.67</v>
       </c>
       <c r="AG37">
@@ -24354,7 +23963,7 @@
         <v>0.36048000000000002</v>
       </c>
       <c r="AI37">
-        <f>AVERAGE(BA7:BD7)</f>
+        <f t="shared" si="0"/>
         <v>9.5431666666666665E-2</v>
       </c>
       <c r="AL37" t="s">
@@ -24414,29 +24023,29 @@
       <c r="M38">
         <v>57060.213192436</v>
       </c>
-      <c r="Q38" s="6">
+      <c r="Q38" s="4">
         <v>30</v>
       </c>
       <c r="R38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1803.77</v>
       </c>
       <c r="S38">
         <v>1</v>
       </c>
       <c r="T38">
+        <f t="shared" si="3"/>
+        <v>36.049999999999997</v>
+      </c>
+      <c r="U38">
         <f t="shared" si="1"/>
-        <v>36.049999999999997</v>
-      </c>
-      <c r="U38">
-        <f>ROUND(AVERAGE(U7:X7),2)</f>
         <v>17.690000000000001</v>
       </c>
       <c r="V38">
         <v>1</v>
       </c>
       <c r="W38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.5399999999999991</v>
       </c>
       <c r="AG38">
@@ -24446,7 +24055,7 @@
         <v>0.40009999999999996</v>
       </c>
       <c r="AI38">
-        <f>AVERAGE(BA8:BD8)</f>
+        <f t="shared" si="0"/>
         <v>0.129995</v>
       </c>
     </row>
@@ -24490,29 +24099,29 @@
       <c r="M39">
         <v>57680.912641848699</v>
       </c>
-      <c r="Q39" s="6">
+      <c r="Q39" s="4">
         <v>40</v>
       </c>
       <c r="R39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1806.15</v>
       </c>
       <c r="S39">
         <v>1</v>
       </c>
       <c r="T39">
+        <f t="shared" si="3"/>
+        <v>40.01</v>
+      </c>
+      <c r="U39">
         <f t="shared" si="1"/>
-        <v>40.01</v>
-      </c>
-      <c r="U39">
-        <f>ROUND(AVERAGE(U8:X8),2)</f>
         <v>20.260000000000002</v>
       </c>
       <c r="V39">
         <v>1</v>
       </c>
       <c r="W39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="AG39">
@@ -24522,7 +24131,7 @@
         <v>0.44114000000000003</v>
       </c>
       <c r="AI39">
-        <f>AVERAGE(BA9:BD9)</f>
+        <f t="shared" si="0"/>
         <v>0.13410666666666668</v>
       </c>
     </row>
@@ -24566,29 +24175,29 @@
       <c r="M40">
         <v>60410.887111936201</v>
       </c>
-      <c r="Q40" s="6">
+      <c r="Q40" s="4">
         <v>50</v>
       </c>
       <c r="R40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1805.13</v>
       </c>
       <c r="S40">
         <v>1</v>
       </c>
       <c r="T40">
+        <f t="shared" si="3"/>
+        <v>44.11</v>
+      </c>
+      <c r="U40">
         <f t="shared" si="1"/>
-        <v>44.11</v>
-      </c>
-      <c r="U40">
-        <f>ROUND(AVERAGE(U9:X9),2)</f>
         <v>21.6</v>
       </c>
       <c r="V40">
         <v>1</v>
       </c>
       <c r="W40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.41</v>
       </c>
       <c r="AG40">
@@ -24598,7 +24207,7 @@
         <v>0.44568000000000002</v>
       </c>
       <c r="AI40">
-        <f>AVERAGE(BA10:BD10)</f>
+        <f t="shared" si="0"/>
         <v>0.16311166666666665</v>
       </c>
       <c r="AM40" t="s">
@@ -24672,29 +24281,29 @@
       <c r="M41">
         <v>59541.296251174899</v>
       </c>
-      <c r="Q41" s="7">
+      <c r="Q41" s="5">
         <v>60</v>
       </c>
       <c r="R41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1805</v>
       </c>
       <c r="S41">
         <v>1</v>
       </c>
       <c r="T41">
+        <f t="shared" si="3"/>
+        <v>44.57</v>
+      </c>
+      <c r="U41">
         <f t="shared" si="1"/>
-        <v>44.57</v>
-      </c>
-      <c r="U41">
-        <f>ROUND(AVERAGE(U10:X10),2)</f>
         <v>26.3</v>
       </c>
       <c r="V41">
         <v>1</v>
       </c>
       <c r="W41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>16.309999999999999</v>
       </c>
       <c r="AG41">
@@ -24704,7 +24313,7 @@
         <v>0.47467999999999994</v>
       </c>
       <c r="AI41">
-        <f>AVERAGE(BA11:BD11)</f>
+        <f t="shared" si="0"/>
         <v>0.17979000000000001</v>
       </c>
       <c r="AK41">
@@ -24794,29 +24403,29 @@
       <c r="M42">
         <v>59541.269303747496</v>
       </c>
-      <c r="Q42" s="7">
+      <c r="Q42" s="5">
         <v>70</v>
       </c>
       <c r="R42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1805.77</v>
       </c>
       <c r="S42">
         <v>1</v>
       </c>
       <c r="T42">
+        <f t="shared" si="3"/>
+        <v>47.47</v>
+      </c>
+      <c r="U42">
         <f t="shared" si="1"/>
-        <v>47.47</v>
-      </c>
-      <c r="U42">
-        <f>ROUND(AVERAGE(U11:X11),2)</f>
         <v>30.34</v>
       </c>
       <c r="V42">
         <v>1</v>
       </c>
       <c r="W42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>17.98</v>
       </c>
       <c r="AG42">
@@ -24826,7 +24435,7 @@
         <v>0.48222000000000004</v>
       </c>
       <c r="AI42">
-        <f>AVERAGE(BA12:BD12)</f>
+        <f t="shared" si="0"/>
         <v>0.19493541666666669</v>
       </c>
       <c r="AU42">
@@ -24902,29 +24511,29 @@
       <c r="M43">
         <v>67103.368192493203</v>
       </c>
-      <c r="Q43" s="7">
+      <c r="Q43" s="5">
         <v>80</v>
       </c>
       <c r="R43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1804.77</v>
       </c>
       <c r="S43">
         <v>1</v>
       </c>
       <c r="T43">
+        <f t="shared" si="3"/>
+        <v>48.22</v>
+      </c>
+      <c r="U43">
         <f t="shared" si="1"/>
-        <v>48.22</v>
-      </c>
-      <c r="U43">
-        <f>ROUND(AVERAGE(U12:X12),2)</f>
         <v>33.78</v>
       </c>
       <c r="V43">
         <v>1</v>
       </c>
       <c r="W43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>19.489999999999998</v>
       </c>
       <c r="AG43">
@@ -24934,7 +24543,7 @@
         <v>0.50578000000000001</v>
       </c>
       <c r="AI43">
-        <f>AVERAGE(BA13:BD13)</f>
+        <f t="shared" si="0"/>
         <v>0.22513333333333335</v>
       </c>
       <c r="AM43" t="s">
@@ -24948,26 +24557,26 @@
       </c>
       <c r="AX43">
         <f ca="1">AVERAGE(AX42,AX45)*(1+RAND()*(1.01-0.99))</f>
-        <v>761.1911048427238</v>
+        <v>761.29067603479257</v>
       </c>
       <c r="AY43">
         <f ca="1">AVERAGE(AY42,AY45)*(1+RAND()*(1.01-0.99))</f>
-        <v>334.5500561075566</v>
+        <v>337.55432743090336</v>
       </c>
       <c r="BA43">
-        <f t="shared" ref="AY43:BD43" si="3">AVERAGE(BA42,BA45)</f>
+        <f t="shared" ref="BA43:BD43" si="5">AVERAGE(BA42,BA45)</f>
         <v>103480.69968253968</v>
       </c>
       <c r="BB43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>338239.52126984129</v>
       </c>
       <c r="BC43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.970208731267137</v>
       </c>
       <c r="BD43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>337.34802633707693</v>
       </c>
     </row>
@@ -25011,29 +24620,29 @@
       <c r="M44">
         <v>51131.1654322635</v>
       </c>
-      <c r="Q44" s="7">
+      <c r="Q44" s="5">
         <v>90</v>
       </c>
       <c r="R44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1805.16</v>
       </c>
       <c r="S44">
         <v>1</v>
       </c>
       <c r="T44">
+        <f t="shared" si="3"/>
+        <v>50.58</v>
+      </c>
+      <c r="U44">
         <f t="shared" si="1"/>
-        <v>50.58</v>
-      </c>
-      <c r="U44">
-        <f>ROUND(AVERAGE(U13:X13),2)</f>
         <v>34.9</v>
       </c>
       <c r="V44">
         <v>1</v>
       </c>
       <c r="W44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>22.51</v>
       </c>
       <c r="AG44">
@@ -25043,7 +24652,7 @@
         <v>0.51888000000000001</v>
       </c>
       <c r="AI44">
-        <f>AVERAGE(BA14:BD14)</f>
+        <f t="shared" si="0"/>
         <v>0.23820166666666667</v>
       </c>
       <c r="AK44">
@@ -25065,26 +24674,26 @@
       </c>
       <c r="AX44">
         <f ca="1">AVERAGE(AX43,AX45)*(1+RAND()*(1.01-0.99))</f>
-        <v>655.718564105067</v>
+        <v>661.00856564196226</v>
       </c>
       <c r="AY44">
-        <f t="shared" ref="AY44:BD44" ca="1" si="4">AVERAGE(AY43,AY45)</f>
-        <v>338.27962343789261</v>
+        <f t="shared" ref="AY44:BD44" ca="1" si="6">AVERAGE(AY43,AY45)</f>
+        <v>339.78175909956599</v>
       </c>
       <c r="BA44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>66015.620952380952</v>
       </c>
       <c r="BB44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>239626.9961904762</v>
       </c>
       <c r="BC44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.4546629122546717</v>
       </c>
       <c r="BD44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>339.42817763680841</v>
       </c>
     </row>
@@ -25128,29 +24737,29 @@
       <c r="M45">
         <v>57307.692274552202</v>
       </c>
-      <c r="Q45" s="7">
+      <c r="Q45" s="5">
         <v>100</v>
       </c>
       <c r="R45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1804.1</v>
       </c>
       <c r="S45">
         <v>1</v>
       </c>
       <c r="T45">
+        <f t="shared" si="3"/>
+        <v>51.89</v>
+      </c>
+      <c r="U45">
         <f t="shared" si="1"/>
-        <v>51.89</v>
-      </c>
-      <c r="U45">
-        <f>ROUND(AVERAGE(U14:X14),2)</f>
         <v>31.9</v>
       </c>
       <c r="V45">
         <v>1</v>
       </c>
       <c r="W45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>23.82</v>
       </c>
       <c r="AU45">
@@ -25237,26 +24846,26 @@
       </c>
       <c r="AX46">
         <f ca="1">AVERAGE(AX45,AX48)*(1+RAND()*(1.01-0.99))</f>
-        <v>396.82687942761652</v>
+        <v>395.54695144232551</v>
       </c>
       <c r="AY46">
         <f ca="1">AVERAGE(AY45,AY48)*(1+RAND()*(1.01-0.99))</f>
-        <v>323.01231482421616</v>
+        <v>318.78964050158135</v>
       </c>
       <c r="BA46">
-        <f t="shared" ref="AY46:BD46" si="5">AVERAGE(BA45,BA48)</f>
+        <f t="shared" ref="BA46:BD46" si="7">AVERAGE(BA45,BA48)</f>
         <v>16832.084846803096</v>
       </c>
       <c r="BB46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>86071.010789686668</v>
       </c>
       <c r="BC46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.5131465516579397</v>
       </c>
       <c r="BD46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>321.89209568935365</v>
       </c>
     </row>
@@ -25341,26 +24950,26 @@
       </c>
       <c r="AX47">
         <f ca="1">AVERAGE(AX46,AX48)</f>
-        <v>321.49431528984513</v>
+        <v>320.85435129719963</v>
       </c>
       <c r="AY47">
-        <f t="shared" ref="AY47:BD47" ca="1" si="6">AVERAGE(AY46,AY48)</f>
-        <v>307.89871172540813</v>
+        <f t="shared" ref="AY47:BD47" ca="1" si="8">AVERAGE(AY46,AY48)</f>
+        <v>305.78737456409067</v>
       </c>
       <c r="BA47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>10972.856159093535</v>
       </c>
       <c r="BB47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>58599.280628974448</v>
       </c>
       <c r="BC47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5.8001612808658063</v>
       </c>
       <c r="BD47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>312.08397906576056</v>
       </c>
     </row>
@@ -25514,27 +25123,27 @@
         <v>20</v>
       </c>
       <c r="R49">
-        <f t="shared" ref="R49:R58" si="7">ROUND(100*AG49,3)</f>
+        <f t="shared" ref="R49:R57" si="9">ROUND(100*AG49,3)</f>
         <v>1.6E-2</v>
       </c>
       <c r="S49">
-        <f t="shared" ref="S49:S57" si="8">ROUND(AH49,2)</f>
+        <f t="shared" ref="S49:S57" si="10">ROUND(AH49,2)</f>
         <v>78770.19</v>
       </c>
       <c r="T49">
-        <f t="shared" ref="T49:W49" si="9">ROUND(BA42,2)</f>
+        <f t="shared" ref="T49:W49" si="11">ROUND(BA42,2)</f>
         <v>178410.86</v>
       </c>
       <c r="U49">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>535464.56999999995</v>
       </c>
       <c r="V49">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="W49">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>333.19</v>
       </c>
       <c r="AG49">
@@ -25562,27 +25171,27 @@
       </c>
       <c r="AX49">
         <f ca="1">AVERAGE(AX48,AX50)*(1+RAND()*(1.01-0.99))</f>
-        <v>197.30257329772817</v>
+        <v>191.53937329816117</v>
       </c>
       <c r="AY49">
         <f ca="1">AVERAGE(AY48,AY50)*(1+RAND()*(1.01-0.99))</f>
-        <v>278.47496056518116</v>
+        <v>280.20515854224931</v>
       </c>
       <c r="BA49">
-        <f t="shared" ref="AZ49:BD49" ca="1" si="10">AVERAGE(BA48,BA50)</f>
-        <v>3020.480108410251</v>
+        <f t="shared" ref="BA49:BD49" ca="1" si="12">AVERAGE(BA48,BA50)</f>
+        <v>3002.0741601825903</v>
       </c>
       <c r="BB49">
-        <f t="shared" ca="1" si="10"/>
-        <v>20036.522096535569</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>19678.327995152322</v>
       </c>
       <c r="BC49">
-        <f t="shared" ca="1" si="10"/>
-        <v>7.8668263565510799</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>7.6639770343654945</v>
       </c>
       <c r="BD49">
-        <f t="shared" ca="1" si="10"/>
-        <v>280.86809470491698</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>280.8680947049171</v>
       </c>
     </row>
     <row r="50" spans="1:56" x14ac:dyDescent="0.2">
@@ -25629,27 +25238,27 @@
         <v>30</v>
       </c>
       <c r="R50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.16400000000000001</v>
       </c>
       <c r="S50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>65194.8</v>
       </c>
       <c r="T50">
-        <f t="shared" ref="T50:W50" si="11">ROUND(BA43,2)</f>
+        <f t="shared" ref="T50:W50" si="13">ROUND(BA43,2)</f>
         <v>103480.7</v>
       </c>
       <c r="U50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>338239.52</v>
       </c>
       <c r="V50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.97</v>
       </c>
       <c r="W50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>337.35</v>
       </c>
       <c r="AG50">
@@ -25669,14 +25278,14 @@
       </c>
       <c r="AV50">
         <f ca="1">AM53/AN53</f>
-        <v>9.6464767030284868</v>
+        <v>9.2407780586573125</v>
       </c>
       <c r="AW50">
         <v>126</v>
       </c>
       <c r="AX50">
         <f ca="1">AM53/AW50</f>
-        <v>143.7668634344289</v>
+        <v>132.25348160425315</v>
       </c>
       <c r="AY50">
         <f>AY48-AY60</f>
@@ -25684,19 +25293,19 @@
       </c>
       <c r="BA50">
         <f ca="1">7840/AW50*(AN53/AW50)</f>
-        <v>927.33274543652772</v>
+        <v>890.52084898120665</v>
       </c>
       <c r="BB50">
         <f ca="1">7840/AW50*AX50</f>
-        <v>8945.49372480891</v>
+        <v>8229.1055220424187</v>
       </c>
       <c r="BC50">
         <f ca="1">BB50/BA50</f>
-        <v>9.646476703028485</v>
+        <v>9.2407780586573143</v>
       </c>
       <c r="BD50">
         <f ca="1">AY50*BC50/AV50</f>
-        <v>259.46032696766662</v>
+        <v>259.46032696766673</v>
       </c>
     </row>
     <row r="51" spans="1:56" x14ac:dyDescent="0.2">
@@ -25743,27 +25352,27 @@
         <v>40</v>
       </c>
       <c r="R51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.35699999999999998</v>
       </c>
       <c r="S51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>60155.4</v>
       </c>
       <c r="T51">
-        <f t="shared" ref="T51:W51" si="12">ROUND(BA44,2)</f>
+        <f t="shared" ref="T51:W51" si="14">ROUND(BA44,2)</f>
         <v>66015.62</v>
       </c>
       <c r="U51">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>239627</v>
       </c>
       <c r="V51">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>4.45</v>
       </c>
       <c r="W51">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>339.43</v>
       </c>
       <c r="AG51">
@@ -25817,27 +25426,27 @@
         <v>50</v>
       </c>
       <c r="R52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.50700000000000001</v>
       </c>
       <c r="S52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>55801.8</v>
       </c>
       <c r="T52">
-        <f t="shared" ref="T52:W52" si="13">ROUND(BA45,2)</f>
+        <f t="shared" ref="T52:W52" si="15">ROUND(BA45,2)</f>
         <v>28550.54</v>
       </c>
       <c r="U52">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>141014.47</v>
       </c>
       <c r="V52">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>4.9400000000000004</v>
       </c>
       <c r="W52">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>341.51</v>
       </c>
       <c r="AG52">
@@ -25901,27 +25510,27 @@
         <v>60</v>
       </c>
       <c r="R53">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.71499999999999997</v>
       </c>
       <c r="S53">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>51713.79</v>
       </c>
       <c r="T53">
-        <f t="shared" ref="T53:W53" si="14">ROUND(BA46,2)</f>
+        <f t="shared" ref="T53:W53" si="16">ROUND(BA46,2)</f>
         <v>16832.080000000002</v>
       </c>
       <c r="U53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>86071.01</v>
       </c>
       <c r="V53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>5.51</v>
       </c>
       <c r="W53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>321.89</v>
       </c>
       <c r="AG53">
@@ -25932,11 +25541,11 @@
       </c>
       <c r="AM53">
         <f ca="1">AM50*(1+RAND()*(0.2))</f>
-        <v>18114.624792738043</v>
+        <v>16663.938682135897</v>
       </c>
       <c r="AN53">
         <f ca="1">AN50/(1+RAND()*0.5)</f>
-        <v>1877.8488095089685</v>
+        <v>1803.3047191869437</v>
       </c>
     </row>
     <row r="54" spans="1:56" x14ac:dyDescent="0.2">
@@ -25983,27 +25592,27 @@
         <v>70</v>
       </c>
       <c r="R54">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.91200000000000003</v>
       </c>
       <c r="S54">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>48289</v>
       </c>
       <c r="T54">
-        <f t="shared" ref="T54:W54" si="15">ROUND(BA47,2)</f>
+        <f t="shared" ref="T54:W54" si="17">ROUND(BA47,2)</f>
         <v>10972.86</v>
       </c>
       <c r="U54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>58599.28</v>
       </c>
       <c r="V54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5.8</v>
       </c>
       <c r="W54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>312.08</v>
       </c>
       <c r="AG54">
@@ -26057,27 +25666,27 @@
         <v>80</v>
       </c>
       <c r="R55">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.94599999999999995</v>
       </c>
       <c r="S55">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>46290.400000000001</v>
       </c>
       <c r="T55">
-        <f t="shared" ref="T55:W55" si="16">ROUND(BA48,2)</f>
+        <f t="shared" ref="T55:W55" si="18">ROUND(BA48,2)</f>
         <v>5113.63</v>
       </c>
       <c r="U55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>31127.55</v>
       </c>
       <c r="V55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>6.09</v>
       </c>
       <c r="W55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>302.27999999999997</v>
       </c>
       <c r="AG55">
@@ -26131,27 +25740,27 @@
         <v>90</v>
       </c>
       <c r="R56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.1759999999999999</v>
       </c>
       <c r="S56">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>43384.6</v>
       </c>
       <c r="T56">
-        <f t="shared" ref="T56:W56" ca="1" si="17">ROUND(BA49,2)</f>
-        <v>3020.48</v>
+        <f t="shared" ref="T56:W56" ca="1" si="19">ROUND(BA49,2)</f>
+        <v>3002.07</v>
       </c>
       <c r="U56">
-        <f t="shared" ca="1" si="17"/>
-        <v>20036.52</v>
+        <f t="shared" ca="1" si="19"/>
+        <v>19678.330000000002</v>
       </c>
       <c r="V56">
-        <f t="shared" ca="1" si="17"/>
-        <v>7.87</v>
+        <f t="shared" ca="1" si="19"/>
+        <v>7.66</v>
       </c>
       <c r="W56">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>280.87</v>
       </c>
       <c r="AG56">
@@ -26205,27 +25814,27 @@
         <v>100</v>
       </c>
       <c r="R57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.361</v>
       </c>
       <c r="S57">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>41014.589999999997</v>
       </c>
       <c r="T57">
-        <f t="shared" ref="T57:W57" ca="1" si="18">ROUND(BA50,2)</f>
-        <v>927.33</v>
+        <f t="shared" ref="T57:W57" ca="1" si="20">ROUND(BA50,2)</f>
+        <v>890.52</v>
       </c>
       <c r="U57">
-        <f t="shared" ca="1" si="18"/>
-        <v>8945.49</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>8229.11</v>
       </c>
       <c r="V57">
-        <f t="shared" ca="1" si="18"/>
-        <v>9.65</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>9.24</v>
       </c>
       <c r="W57">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="20"/>
         <v>259.45999999999998</v>
       </c>
       <c r="AG57">

</xml_diff>